<commit_message>
wieder mal wunderbarer code
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -101,76 +101,76 @@
               <c:numCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>4531465.2</c:v>
+                  <c:v>1746222.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2529060.9</c:v>
+                  <c:v>852565.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>737256.4</c:v>
+                  <c:v>254353.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295407.9</c:v>
+                  <c:v>110736.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>240647.8</c:v>
+                  <c:v>57767.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158691.9</c:v>
+                  <c:v>31158.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51018.8</c:v>
+                  <c:v>15566.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13870.7</c:v>
+                  <c:v>8341.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5512.8</c:v>
+                  <c:v>4252.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5324.9</c:v>
+                  <c:v>2525.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2640.8</c:v>
+                  <c:v>1087.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1218.1</c:v>
+                  <c:v>538.1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>637.9</c:v>
+                  <c:v>281.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>183.6</c:v>
+                  <c:v>152.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>95.3</c:v>
+                  <c:v>80.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>61.0</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43.7</c:v>
+                  <c:v>24.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.9</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.2</c:v>
+                  <c:v>21.3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16.4</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.5</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18.6</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -231,7 +231,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Duration</a:t>
+                  <a:t>Duration in Microseconds</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
@@ -318,7 +318,7 @@
         <v>8.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4531465.2</v>
+        <v>1746222.9</v>
       </c>
     </row>
     <row r="3">
@@ -326,7 +326,7 @@
         <v>9.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>2529060.9</v>
+        <v>852565.1</v>
       </c>
     </row>
     <row r="4">
@@ -334,7 +334,7 @@
         <v>10.0</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>737256.4</v>
+        <v>254353.3</v>
       </c>
     </row>
     <row r="5">
@@ -342,7 +342,7 @@
         <v>11.0</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>295407.9</v>
+        <v>110736.2</v>
       </c>
     </row>
     <row r="6">
@@ -350,7 +350,7 @@
         <v>12.0</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>240647.8</v>
+        <v>57767.7</v>
       </c>
     </row>
     <row r="7">
@@ -358,7 +358,7 @@
         <v>13.0</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>158691.9</v>
+        <v>31158.9</v>
       </c>
     </row>
     <row r="8">
@@ -366,7 +366,7 @@
         <v>14.0</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>51018.8</v>
+        <v>15566.6</v>
       </c>
     </row>
     <row r="9">
@@ -374,7 +374,7 @@
         <v>15.0</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>13870.7</v>
+        <v>8341.4</v>
       </c>
     </row>
     <row r="10">
@@ -382,7 +382,7 @@
         <v>16.0</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>5512.8</v>
+        <v>4252.6</v>
       </c>
     </row>
     <row r="11">
@@ -390,7 +390,7 @@
         <v>17.0</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>5324.9</v>
+        <v>2525.6</v>
       </c>
     </row>
     <row r="12">
@@ -398,7 +398,7 @@
         <v>18.0</v>
       </c>
       <c r="B12" t="n" s="0">
-        <v>2640.8</v>
+        <v>1087.1</v>
       </c>
     </row>
     <row r="13">
@@ -406,7 +406,7 @@
         <v>19.0</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>1218.1</v>
+        <v>538.1</v>
       </c>
     </row>
     <row r="14">
@@ -414,7 +414,7 @@
         <v>20.0</v>
       </c>
       <c r="B14" t="n" s="0">
-        <v>637.9</v>
+        <v>281.7</v>
       </c>
     </row>
     <row r="15">
@@ -422,7 +422,7 @@
         <v>21.0</v>
       </c>
       <c r="B15" t="n" s="0">
-        <v>183.6</v>
+        <v>152.1</v>
       </c>
     </row>
     <row r="16">
@@ -430,7 +430,7 @@
         <v>22.0</v>
       </c>
       <c r="B16" t="n" s="0">
-        <v>95.3</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="17">
@@ -438,7 +438,7 @@
         <v>23.0</v>
       </c>
       <c r="B17" t="n" s="0">
-        <v>61.0</v>
+        <v>42.7</v>
       </c>
     </row>
     <row r="18">
@@ -446,7 +446,7 @@
         <v>24.0</v>
       </c>
       <c r="B18" t="n" s="0">
-        <v>43.7</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="19">
@@ -454,7 +454,7 @@
         <v>25.0</v>
       </c>
       <c r="B19" t="n" s="0">
-        <v>26.9</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="20">
@@ -462,7 +462,7 @@
         <v>26.0</v>
       </c>
       <c r="B20" t="n" s="0">
-        <v>19.2</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="21">
@@ -470,7 +470,7 @@
         <v>27.0</v>
       </c>
       <c r="B21" t="n" s="0">
-        <v>16.4</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="22">
@@ -478,7 +478,7 @@
         <v>28.0</v>
       </c>
       <c r="B22" t="n" s="0">
-        <v>14.5</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="23">
@@ -486,7 +486,7 @@
         <v>29.0</v>
       </c>
       <c r="B23" t="n" s="0">
-        <v>14.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="24">
@@ -494,7 +494,7 @@
         <v>30.0</v>
       </c>
       <c r="B24" t="n" s="0">
-        <v>13.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="25">
@@ -502,7 +502,7 @@
         <v>31.0</v>
       </c>
       <c r="B25" t="n" s="0">
-        <v>18.6</v>
+        <v>6.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>